<commit_message>
new server version 2.0
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evgen\OneDrive\Рабочий стол\Тесты стратегий\черновики\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Symbol</t>
   </si>
@@ -119,7 +114,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -464,7 +459,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -475,21 +470,21 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -541,22 +536,22 @@
         <v>13</v>
       </c>
       <c r="E2" s="3">
-        <v>5.0999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="F2" s="3">
         <v>90</v>
       </c>
       <c r="G2" s="3">
-        <v>9</v>
+        <v>0.25</v>
       </c>
       <c r="H2" s="3">
         <v>10</v>
       </c>
       <c r="I2" s="3">
-        <v>9.1</v>
+        <v>1</v>
       </c>
       <c r="J2" s="3">
-        <v>2</v>
+        <v>0.05</v>
       </c>
       <c r="K2" s="3">
         <v>2</v>
@@ -576,22 +571,22 @@
         <v>13</v>
       </c>
       <c r="E3" s="3">
-        <v>4.5999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="F3" s="3">
         <v>50</v>
       </c>
       <c r="G3" s="3">
-        <v>8.5</v>
+        <v>0.5</v>
       </c>
       <c r="H3" s="3">
         <v>50</v>
       </c>
       <c r="I3" s="3">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="J3" s="3">
-        <v>2.2000000000000002</v>
+        <v>0.05</v>
       </c>
       <c r="K3" s="3">
         <v>1</v>
@@ -891,22 +886,22 @@
         <v>13</v>
       </c>
       <c r="E12" s="3">
-        <v>4</v>
+        <v>0.2</v>
       </c>
       <c r="F12" s="3">
         <v>50</v>
       </c>
       <c r="G12" s="3">
-        <v>8</v>
+        <v>0.8</v>
       </c>
       <c r="H12" s="3">
         <v>50</v>
       </c>
       <c r="I12" s="3">
-        <v>4</v>
+        <v>0.9</v>
       </c>
       <c r="J12" s="3">
-        <v>2</v>
+        <v>0.05</v>
       </c>
       <c r="K12" s="3">
         <v>1</v>
@@ -932,7 +927,7 @@
         <v>50</v>
       </c>
       <c r="G13" s="3">
-        <v>8</v>
+        <v>0.4</v>
       </c>
       <c r="H13" s="3">
         <v>50</v>
@@ -966,8 +961,8 @@
       <c r="F14" s="3">
         <v>100</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>12</v>
+      <c r="G14" s="3">
+        <v>0.4</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>12</v>
@@ -1002,7 +997,7 @@
         <v>80</v>
       </c>
       <c r="G15" s="3">
-        <v>15</v>
+        <v>0.4</v>
       </c>
       <c r="H15" s="3">
         <v>20</v>
@@ -1037,7 +1032,7 @@
         <v>50</v>
       </c>
       <c r="G16" s="3">
-        <v>16</v>
+        <v>0.4</v>
       </c>
       <c r="H16" s="3">
         <v>50</v>
@@ -1071,8 +1066,8 @@
       <c r="F17" s="3">
         <v>100</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>12</v>
+      <c r="G17" s="3">
+        <v>0.4</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>12</v>

</xml_diff>